<commit_message>
for wanglei to pull sync
</commit_message>
<xml_diff>
--- a/document/网站模块设计/危废管理系统网站模块设计.xlsx
+++ b/document/网站模块设计/危废管理系统网站模块设计.xlsx
@@ -670,11 +670,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1070,7 +1070,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1081,7 +1081,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1090,7 +1090,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1099,7 +1099,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1108,7 +1108,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1126,28 +1126,28 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1197,16 +1197,16 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
         <v>75</v>
       </c>
@@ -1568,7 +1568,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="3"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="3"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="5" t="s">
         <v>77</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="3"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="1" t="s">
@@ -1605,7 +1605,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="3"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="1" t="s">
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="3"/>
+      <c r="A36" s="4"/>
       <c r="B36" s="5" t="s">
         <v>76</v>
       </c>
@@ -1631,7 +1631,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="3"/>
+      <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="1" t="s">
@@ -1642,7 +1642,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="3"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="5" t="s">
         <v>78</v>
       </c>
@@ -1657,7 +1657,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="3"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="1" t="s">
@@ -1668,7 +1668,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1685,7 +1685,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="3"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="5" t="s">
         <v>39</v>
       </c>
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="3"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1" t="s">
@@ -1711,7 +1711,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="3"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="5" t="s">
         <v>100</v>
       </c>
@@ -1726,7 +1726,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="3"/>
+      <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="1" t="s">
@@ -1737,7 +1737,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="3"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="5" t="s">
         <v>101</v>
       </c>
@@ -1752,7 +1752,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="3"/>
+      <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="1" t="s">
@@ -1763,7 +1763,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1780,7 +1780,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="3"/>
+      <c r="A48" s="4"/>
       <c r="B48" s="5" t="s">
         <v>39</v>
       </c>
@@ -1795,7 +1795,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="3"/>
+      <c r="A49" s="4"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="1" t="s">
@@ -1806,7 +1806,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="3"/>
+      <c r="A50" s="4"/>
       <c r="B50" s="5" t="s">
         <v>115</v>
       </c>
@@ -1821,7 +1821,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="3"/>
+      <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="1" t="s">
@@ -1832,7 +1832,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="3"/>
+      <c r="A52" s="4"/>
       <c r="B52" s="5" t="s">
         <v>100</v>
       </c>
@@ -1847,7 +1847,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="3"/>
+      <c r="A53" s="4"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="1" t="s">
@@ -1859,42 +1859,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="A2:A29"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B18:B29"/>
+    <mergeCell ref="C18:C29"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B18:B29"/>
-    <mergeCell ref="C18:C29"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="A2:A29"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A30:A39"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A47:A53"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add content of country's sidebar and ajax
</commit_message>
<xml_diff>
--- a/document/网站模块设计/危废管理系统网站模块设计.xlsx
+++ b/document/网站模块设计/危废管理系统网站模块设计.xlsx
@@ -237,10 +237,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>statistic_analysis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>business</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -602,6 +598,10 @@
   </si>
   <si>
     <t>reception_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transfer_statistic_analysis</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1198,28 +1198,28 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>36</v>
@@ -1370,7 +1370,7 @@
         <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -1379,13 +1379,13 @@
         <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -1393,10 +1393,10 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -1405,13 +1405,13 @@
         <v>19</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -1419,10 +1419,10 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -1430,10 +1430,10 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -1441,10 +1441,10 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -1452,10 +1452,10 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -1463,10 +1463,10 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -1474,10 +1474,10 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -1485,10 +1485,10 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -1496,10 +1496,10 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -1507,10 +1507,10 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -1518,10 +1518,10 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -1529,36 +1529,36 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D30" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>39</v>
@@ -1572,25 +1572,25 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
       <c r="B33" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -1598,10 +1598,10 @@
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -1609,25 +1609,25 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="4"/>
       <c r="B36" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -1635,25 +1635,25 @@
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="4"/>
       <c r="B38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -1661,27 +1661,27 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -1690,7 +1690,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>39</v>
@@ -1704,25 +1704,25 @@
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="4"/>
       <c r="B43" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -1730,25 +1730,25 @@
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="4"/>
       <c r="B45" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
@@ -1756,27 +1756,27 @@
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
@@ -1785,13 +1785,13 @@
         <v>39</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
@@ -1799,25 +1799,25 @@
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="4"/>
       <c r="B50" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="D50" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
@@ -1825,25 +1825,25 @@
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="4"/>
       <c r="B52" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
@@ -1851,33 +1851,15 @@
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A47:A53"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="C13:C15"/>
     <mergeCell ref="A2:A29"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
@@ -1894,7 +1876,25 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>